<commit_message>
Restricted and view users cannot access Delete/DeleteConfirmed routes.
</commit_message>
<xml_diff>
--- a/Documentation/Test Plan.xlsx
+++ b/Documentation/Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\aimee-craig-sp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63A4F92-10FB-4BC7-8EAF-0FD8190D0E07}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDA284B-868F-44DA-AE9A-10863E8F316E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" xr2:uid="{93FAF29C-E983-4090-91B7-3E30D4B66AF4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="63">
   <si>
     <t>Tester's Name</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>"Delete Quiz" button is visible</t>
+  </si>
+  <si>
+    <t>Restricted user navigates to /Quizzes/Delete</t>
+  </si>
+  <si>
+    <t>View user navigates to /Quizzes/Delete</t>
+  </si>
+  <si>
+    <t>Restricted user navigates to /Quizzes/DeleteConfirmed</t>
+  </si>
+  <si>
+    <t>View user navigates to /Quizzes/DeleteConfirmed</t>
   </si>
 </sst>
 </file>
@@ -625,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E3D155-EA1A-42E2-9565-5B23BCA31E22}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1189,6 +1201,86 @@
         <v>10</v>
       </c>
       <c r="F29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added edit button to quiz cards.
</commit_message>
<xml_diff>
--- a/Documentation/Test Plan.xlsx
+++ b/Documentation/Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\aimee-craig-sp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893EA85E-DB15-4CED-9763-1D108BB2C6E5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65705A3F-CA9C-4CD0-B551-5C1BD9AED46D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" xr2:uid="{93FAF29C-E983-4090-91B7-3E30D4B66AF4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="67">
   <si>
     <t>Tester's Name</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>View user navigates to /Quizzes/Edit</t>
+  </si>
+  <si>
+    <t>"Edit Quiz" button is not visible</t>
+  </si>
+  <si>
+    <t>"Edit Quiz" button is visible</t>
   </si>
 </sst>
 </file>
@@ -287,7 +293,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -643,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E3D155-EA1A-42E2-9565-5B23BCA31E22}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1330,8 +1376,82 @@
         <v>11</v>
       </c>
     </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F4:F1048576">
+  <conditionalFormatting sqref="F4:F35 F39:F1048576">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"Suspended"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"Not Executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36:F38">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Suspended"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Users must be authenticated to access web app.
</commit_message>
<xml_diff>
--- a/Documentation/Test Plan.xlsx
+++ b/Documentation/Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\aimee-craig-sp\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E55665-D424-4FA1-8E6B-A9EFA43555F4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6EB0DE-C86E-4550-B8EE-6315E83AE6CC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16749" xr2:uid="{93FAF29C-E983-4090-91B7-3E30D4B66AF4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="80">
   <si>
     <t>Tester's Name</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Successful login</t>
   </si>
   <si>
-    <t>User is redirected to https://localhost:44302/</t>
-  </si>
-  <si>
     <t>Same as expected</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Unsuccessful login</t>
   </si>
   <si>
-    <t>User remains on https://localhost:44302/Account/Login</t>
-  </si>
-  <si>
     <t>Area</t>
   </si>
   <si>
@@ -105,9 +99,6 @@
     <t>User logs out</t>
   </si>
   <si>
-    <t>User is redirected to https://localhost:44302/Account/Login</t>
-  </si>
-  <si>
     <t>View Quiz</t>
   </si>
   <si>
@@ -259,6 +250,27 @@
   </si>
   <si>
     <t>"Add Answer" button for that question is enabled</t>
+  </si>
+  <si>
+    <t>Unauthenticated user navigates to /Quizzes/Create</t>
+  </si>
+  <si>
+    <t>Unauthenticated user navigates to /Quizzes/Details?id=1</t>
+  </si>
+  <si>
+    <t>Unauthenticated user navigates to /Quizzes/Edit?id=1</t>
+  </si>
+  <si>
+    <t>Unauthenticated user navigates to /Quizzes/Delete?id=1</t>
+  </si>
+  <si>
+    <t>User is redirected to /Account/Login</t>
+  </si>
+  <si>
+    <t>User is redirected to /Quizzes/Index</t>
+  </si>
+  <si>
+    <t>User remains on /Account/Login</t>
   </si>
 </sst>
 </file>
@@ -796,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E3D155-EA1A-42E2-9565-5B23BCA31E22}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -828,7 +840,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -843,44 +855,44 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -888,19 +900,19 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -908,19 +920,19 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="58.3" x14ac:dyDescent="0.4">
@@ -928,19 +940,19 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">
@@ -948,39 +960,39 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.4">
@@ -988,19 +1000,19 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
@@ -1008,19 +1020,19 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.4">
@@ -1028,19 +1040,19 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.4">
@@ -1048,19 +1060,19 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.4">
@@ -1068,19 +1080,19 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
@@ -1088,19 +1100,19 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.4">
@@ -1108,19 +1120,19 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
@@ -1128,19 +1140,19 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1148,19 +1160,19 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
@@ -1168,19 +1180,19 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1188,19 +1200,19 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.75" x14ac:dyDescent="0.4">
@@ -1208,19 +1220,19 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1228,19 +1240,19 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1248,19 +1260,19 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1268,19 +1280,19 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
@@ -1288,19 +1300,19 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
@@ -1308,19 +1320,19 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
@@ -1328,19 +1340,19 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
@@ -1348,19 +1360,19 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1368,19 +1380,19 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
@@ -1388,19 +1400,19 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1408,19 +1420,19 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1428,19 +1440,19 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
@@ -1448,19 +1460,19 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.4">
@@ -1468,19 +1480,19 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.4">
@@ -1488,19 +1500,19 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.4">
@@ -1508,19 +1520,19 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.4">
@@ -1528,19 +1540,19 @@
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1548,19 +1560,19 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.75" x14ac:dyDescent="0.4">
@@ -1568,19 +1580,19 @@
         <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1588,19 +1600,19 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1608,19 +1620,19 @@
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1628,19 +1640,19 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.4">
@@ -1648,19 +1660,19 @@
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1668,19 +1680,19 @@
         <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1688,19 +1700,19 @@
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1708,19 +1720,19 @@
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1728,19 +1740,19 @@
         <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1748,19 +1760,19 @@
         <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1768,19 +1780,19 @@
         <v>47</v>
       </c>
       <c r="B50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="D50" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1788,19 +1800,19 @@
         <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
@@ -1808,23 +1820,103 @@
         <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E52" t="s">
-        <v>10</v>
-      </c>
-      <c r="F52" t="s">
-        <v>11</v>
+      <c r="D55" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F4:F35 F45:F48 F53:F1048576">
+  <conditionalFormatting sqref="F4:F35 F45:F48 F57:F1048576">
     <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Suspended"</formula>
     </cfRule>
@@ -1866,7 +1958,7 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F49:F52">
+  <conditionalFormatting sqref="F49:F56">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Suspended"</formula>
     </cfRule>

</xml_diff>